<commit_message>
SpringSecurity & FileUpload OK 2
</commit_message>
<xml_diff>
--- a/Player-TEST.xlsx
+++ b/Player-TEST.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>EMAIL_ADDRESS</t>
   </si>
@@ -109,7 +109,34 @@
     <t>ROLES</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>OPERATOR</t>
+  </si>
+  <si>
+    <t>Luka</t>
+  </si>
+  <si>
+    <t>Doncic</t>
+  </si>
+  <si>
+    <t>luka.doncic@me.com</t>
+  </si>
+  <si>
+    <t>dsjhds@fdkfjdk.com</t>
+  </si>
+  <si>
+    <t>dfd0#sdsf</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>as</t>
   </si>
 </sst>
 </file>
@@ -471,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,7 +570,10 @@
         <v>17</v>
       </c>
       <c r="E2" s="4">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
       </c>
       <c r="G2" s="3">
         <v>30247</v>
@@ -578,7 +608,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="4">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -599,7 +629,7 @@
         <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -616,7 +646,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="4">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
@@ -637,7 +667,83 @@
         <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H5" s="4">
+        <v>110</v>
+      </c>
+      <c r="I5" s="4">
+        <v>205</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3">
+        <v>28755</v>
+      </c>
+      <c r="H6" s="4">
+        <v>90</v>
+      </c>
+      <c r="I6" s="4">
+        <v>198</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -645,8 +751,10 @@
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SpringSecurity & FileUpload OK 3
</commit_message>
<xml_diff>
--- a/Player-TEST.xlsx
+++ b/Player-TEST.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>EMAIL_ADDRESS</t>
   </si>
@@ -85,9 +85,6 @@
     <t>NATIONALITY</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
   </si>
   <si>
     <t>dfd0#sdsf</t>
-  </si>
-  <si>
-    <t>sa</t>
   </si>
   <si>
     <t>as</t>
@@ -501,7 +495,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,10 +544,10 @@
         <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -566,15 +560,9 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
       <c r="G2" s="3">
         <v>30247</v>
       </c>
@@ -584,14 +572,11 @@
       <c r="I2" s="4">
         <v>185</v>
       </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -623,13 +608,13 @@
         <v>198</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -661,24 +646,24 @@
         <v>205</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -699,13 +684,13 @@
         <v>205</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -716,7 +701,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -725,7 +710,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="3">
         <v>28755</v>
@@ -737,13 +722,13 @@
         <v>198</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>